<commit_message>
Ajustes Cadastro, Busca e Exclusão
</commit_message>
<xml_diff>
--- a/output/database.xlsx
+++ b/output/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
@@ -79,12 +79,8 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -100,10 +96,10 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -452,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -464,22 +460,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Username</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Tipo</t>
         </is>
@@ -574,8 +570,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -590,6 +588,26 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>kelly</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kelly</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -604,10 +622,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -619,27 +637,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>RG</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Data de Nascimento</t>
         </is>
@@ -754,8 +772,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -775,6 +795,31 @@
       <c r="E6" t="inlineStr">
         <is>
           <t>11/01/2001</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Kelly dos Santos</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>457244195</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>98765432</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>02/04/2005</t>
         </is>
       </c>
     </row>
@@ -789,9 +834,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -801,27 +846,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>RG</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Data de Nascimento</t>
         </is>
@@ -851,6 +896,85 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>98765</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>01/01/2001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Millenao</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>888123775</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>66123554</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>09/10/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>aitavarinhopvp</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1138007736</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>72653467</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>19/09/2002</t>
         </is>
       </c>
     </row>
@@ -865,15 +989,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="10.6328125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.90625" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -897,6 +1022,11 @@
           <t>Preco</t>
         </is>
       </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Tipo de Venda</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -919,6 +1049,7 @@
           <t>5</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -931,12 +1062,107 @@
           <t>Banana</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>100</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>2.75</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Super Morangao</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bergamota</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3.98</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Granel</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Kiwi</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Peso</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementaçao sistema de caixa
</commit_message>
<xml_diff>
--- a/output/database.xlsx
+++ b/output/database.xlsx
@@ -79,8 +79,12 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -96,10 +100,10 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -448,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -460,22 +464,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Username</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Tipo</t>
         </is>
@@ -592,8 +596,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -608,6 +614,26 @@
       <c r="D7" t="inlineStr">
         <is>
           <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>le</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>le</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -622,7 +648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -637,27 +663,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>RG</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Data de Nascimento</t>
         </is>
@@ -799,8 +825,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -820,6 +848,31 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>02/04/2005</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>leticia</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-327372859</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>576681301</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>16/03/2006</t>
         </is>
       </c>
     </row>
@@ -992,7 +1045,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1049,7 +1102,11 @@
           <t>5</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Granel</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1072,7 +1129,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Peso</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1095,70 +1156,82 @@
           <t>4.5</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Peso</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bergamota</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>3.98</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Granel</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bergamota</t>
+          <t>Kiwi</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>80</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.98</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Granel</t>
+          <t>Peso</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Morango</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Kiwi</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1.25</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Ajustes controle de estoque
</commit_message>
<xml_diff>
--- a/output/database.xlsx
+++ b/output/database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
@@ -33,7 +33,9 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,16 +70,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -86,6 +97,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +449,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="9.36328125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9.36328125" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -657,10 +669,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="19.453125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="11.81640625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="9.81640625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="17.7265625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="19.453125" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="11.81640625" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="9.81640625" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
+    <col width="17.7265625" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -919,13 +931,13 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="17.7265625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="17.7265625" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1022,14 +1034,14 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="10.6328125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="12.90625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="10.6328125" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="12.90625" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1072,7 +1084,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1099,7 +1111,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>100.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1126,7 +1138,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>80.0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1153,7 +1165,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>45.0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1180,7 +1192,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>80.0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1207,7 +1219,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1234,7 +1246,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>177.3</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1259,11 +1271,13 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>70</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>2.39</v>
+          <t>70.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1273,5 +1287,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>